<commit_message>
Arranged some of the data files and folders
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Diagram_Creator\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Diagram_Creator\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CAF818-4E75-4336-A15B-37449CA83118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0E887-D97A-4FD9-9383-7744BEF4173F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27600" yWindow="420" windowWidth="26640" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1140,18 +1140,9 @@
     <t>Stencil</t>
   </si>
   <si>
-    <t>C:\Omnicell_Diagram_Creator\Stencils\OC_ArchitectStencils.vssx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Diagram_Creator\Stencils\Advocate_CustomStencils.vssx</t>
-  </si>
-  <si>
     <t>;0</t>
   </si>
   <si>
-    <t>C:\Omnicell_Diagram_Creator\Templates\OC_ArchitectDiagramTemplate.vstx</t>
-  </si>
-  <si>
     <t>; Visio Sec tion</t>
   </si>
   <si>
@@ -1171,6 +1162,15 @@
   </si>
   <si>
     <t>Blank Document</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Diagram_Creator\Data\Templates\OC_ArchitectDiagramTemplate.vstx</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Diagram_Creator\Data\Stencils\OC_ArchitectStencils.vssx</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Diagram_Creator\Data\Stencils\Advocate_CustomStencils.vssx</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2312,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,17 +2486,17 @@
     </row>
     <row r="3" spans="1:32" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>291</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
@@ -2547,12 +2547,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
       <c r="E4" s="44" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -2606,11 +2606,11 @@
         <v>292</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="AF5" s="25"/>
     </row>
-    <row r="6" spans="1:32" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="43">
         <v>0</v>
       </c>
@@ -2664,11 +2664,11 @@
         <v>292</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Changed the application name to Omnicell Blueprinting Tool change the folder to OmnicellBlueprintingTool changed the Template and Stencil names
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Diagram_Creator\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB0E887-D97A-4FD9-9383-7744BEF4173F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998E309-A166-4B08-8F31-D47E47D805C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="420" windowWidth="26640" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3570" yWindow="900" windowWidth="27375" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -1164,13 +1164,13 @@
     <t>Blank Document</t>
   </si>
   <si>
-    <t>C:\Omnicell_Diagram_Creator\Data\Templates\OC_ArchitectDiagramTemplate.vstx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Diagram_Creator\Data\Stencils\OC_ArchitectStencils.vssx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Diagram_Creator\Data\Stencils\Advocate_CustomStencils.vssx</t>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Advocate_CustomStencils.vssx</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2312,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="AF4" s="25"/>
     </row>
-    <row r="5" spans="1:32" s="27" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>0</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>292</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
@@ -2664,7 +2664,7 @@
         <v>292</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44" t="s">

</xml_diff>

<commit_message>
Finishing touches on the User Guide.  Saved in latest word version.  Updated the blueprinting data file template.
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F998E309-A166-4B08-8F31-D47E47D805C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F81C47-41CC-461B-A266-20FFA3A17028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="900" windowWidth="27375" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18840" yWindow="300" windowWidth="27375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="305">
   <si>
     <t>Shape</t>
   </si>
@@ -804,52 +804,7 @@
     <t>Connect From</t>
   </si>
   <si>
-    <t>From LineLabel</t>
-  </si>
-  <si>
-    <t>From LinePattern</t>
-  </si>
-  <si>
-    <t>From ArrowType</t>
-  </si>
-  <si>
-    <t>From LineColor</t>
-  </si>
-  <si>
     <t>Connect To</t>
-  </si>
-  <si>
-    <t>To LineLabel</t>
-  </si>
-  <si>
-    <t>To LinePattern</t>
-  </si>
-  <si>
-    <t>To ArrowType</t>
-  </si>
-  <si>
-    <t>To LineColor</t>
-  </si>
-  <si>
-    <t>mach name</t>
-  </si>
-  <si>
-    <t>mach id</t>
-  </si>
-  <si>
-    <t>site id</t>
-  </si>
-  <si>
-    <t>site name</t>
-  </si>
-  <si>
-    <t>site address</t>
-  </si>
-  <si>
-    <t>omnis name</t>
-  </si>
-  <si>
-    <t>omnis id</t>
   </si>
   <si>
     <t>site_id omnis_id</t>
@@ -1171,6 +1126,54 @@
   </si>
   <si>
     <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
+  </si>
+  <si>
+    <t>Shape Label Font Size</t>
+  </si>
+  <si>
+    <t>From Line Label</t>
+  </si>
+  <si>
+    <t>From Line Pattern</t>
+  </si>
+  <si>
+    <t>From Arrow Type</t>
+  </si>
+  <si>
+    <t>From Line Color</t>
+  </si>
+  <si>
+    <t>To Line Label</t>
+  </si>
+  <si>
+    <t>To Line Pattern</t>
+  </si>
+  <si>
+    <t>To Arrow Type</t>
+  </si>
+  <si>
+    <t>To Line Color</t>
+  </si>
+  <si>
+    <t>mach_name</t>
+  </si>
+  <si>
+    <t>mach_id</t>
+  </si>
+  <si>
+    <t>site_id</t>
+  </si>
+  <si>
+    <t>site_name</t>
+  </si>
+  <si>
+    <t>site_address</t>
+  </si>
+  <si>
+    <t>omnis_name</t>
+  </si>
+  <si>
+    <t>omnis_id</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2315,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,16 +2326,16 @@
     <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="6.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="3" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="3" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="2" customWidth="1"/>
+    <col min="8" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
     <col min="18" max="19" width="9.140625" style="4"/>
     <col min="20" max="20" width="12.140625" style="4" customWidth="1"/>
     <col min="21" max="21" width="8.7109375" style="4" customWidth="1"/>
@@ -2352,7 +2355,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>181</v>
@@ -2367,31 +2370,31 @@
         <v>184</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>185</v>
+        <v>289</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>198</v>
+        <v>298</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>199</v>
+        <v>299</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>201</v>
+        <v>301</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>202</v>
+        <v>302</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>203</v>
+        <v>303</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>204</v>
+        <v>304</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>17</v>
@@ -2421,36 +2424,36 @@
         <v>188</v>
       </c>
       <c r="X1" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y1" s="35" t="s">
+        <v>291</v>
+      </c>
+      <c r="Z1" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="AA1" s="35" t="s">
+        <v>293</v>
+      </c>
+      <c r="AB1" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="Y1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="Z1" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="AA1" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>193</v>
-      </c>
       <c r="AC1" s="36" t="s">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="AD1" s="36" t="s">
-        <v>195</v>
+        <v>295</v>
       </c>
       <c r="AE1" s="36" t="s">
-        <v>196</v>
+        <v>296</v>
       </c>
       <c r="AF1" s="36" t="s">
-        <v>197</v>
+        <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -2486,17 +2489,17 @@
     </row>
     <row r="3" spans="1:32" s="27" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
@@ -2547,12 +2550,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
       <c r="E4" s="44" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="23"/>
@@ -2603,14 +2606,14 @@
         <v>0</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C5" s="48" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -2661,14 +2664,14 @@
         <v>0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="23"/>
@@ -2716,7 +2719,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2816,22 +2819,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
@@ -2886,7 +2889,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="F10" s="23">
         <v>9</v>
@@ -3067,7 +3070,7 @@
         <v>0</v>
       </c>
       <c r="V13" s="26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="W13" s="23"/>
       <c r="X13" s="25"/>
@@ -3133,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="V14" s="26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="W14" s="23"/>
       <c r="X14" s="25"/>
@@ -3199,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="W15" s="23" t="s">
         <v>58</v>
@@ -3271,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="V16" s="26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="W16" s="23"/>
       <c r="X16" s="25"/>
@@ -3337,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="26" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="W17" s="25" t="s">
         <v>58</v>
@@ -3377,7 +3380,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -3790,7 +3793,7 @@
         <v>34</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
@@ -3845,7 +3848,7 @@
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -3892,7 +3895,7 @@
         <v>40</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
@@ -4184,13 +4187,13 @@
         <v>0</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F32" s="23" t="s">
         <v>177</v>
@@ -4288,7 +4291,7 @@
         <v>89</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="F34" s="23" t="s">
         <v>177</v>
@@ -4418,7 +4421,7 @@
         <v>18</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="23"/>
@@ -4482,7 +4485,7 @@
         <v>18</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
@@ -4708,13 +4711,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>89</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F41" s="23" t="s">
         <v>177</v>
@@ -4776,7 +4779,7 @@
         <v>50</v>
       </c>
       <c r="E42" s="23" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
@@ -4844,7 +4847,7 @@
         <v>50</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
@@ -5074,7 +5077,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="F47" s="23"/>
       <c r="G47" s="23"/>
@@ -5134,7 +5137,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="F48" s="34">
         <v>10</v>
@@ -5292,7 +5295,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="23"/>
@@ -6132,7 +6135,7 @@
         <v>7</v>
       </c>
       <c r="E65" s="19" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
@@ -6196,7 +6199,7 @@
         <v>10</v>
       </c>
       <c r="E66" s="19" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F66" s="19"/>
       <c r="G66" s="19"/>
@@ -6254,13 +6257,13 @@
         <v>0</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="D67" s="23" t="s">
         <v>89</v>
       </c>
       <c r="E67" s="23" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F67" s="23"/>
       <c r="G67" s="23"/>
@@ -7726,7 +7729,7 @@
         <v>7</v>
       </c>
       <c r="E92" s="19" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="F92" s="19"/>
       <c r="G92" s="19"/>
@@ -7790,7 +7793,7 @@
         <v>10</v>
       </c>
       <c r="E93" s="19" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="F93" s="19"/>
       <c r="G93" s="19"/>
@@ -7848,13 +7851,13 @@
         <v>0</v>
       </c>
       <c r="C94" s="23" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="D94" s="23" t="s">
         <v>89</v>
       </c>
       <c r="E94" s="23" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="F94" s="23"/>
       <c r="G94" s="23"/>
@@ -8478,7 +8481,7 @@
     </row>
     <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
@@ -8520,13 +8523,13 @@
         <v>0</v>
       </c>
       <c r="C106" s="44" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="D106" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E106" s="45" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="F106" s="45">
         <v>8</v>
@@ -8582,13 +8585,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="44" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="D107" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E107" s="45" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="F107" s="45">
         <v>8</v>
@@ -8644,13 +8647,13 @@
         <v>0</v>
       </c>
       <c r="C108" s="44" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="D108" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E108" s="45" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="F108" s="45">
         <v>8</v>
@@ -8706,13 +8709,13 @@
         <v>0</v>
       </c>
       <c r="C109" s="23" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="D109" s="23" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E109" s="34" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="F109" s="34">
         <v>8</v>
@@ -8766,13 +8769,13 @@
         <v>0</v>
       </c>
       <c r="C110" s="23" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="D110" s="23" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E110" s="34" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F110" s="34">
         <v>8</v>
@@ -8826,13 +8829,13 @@
         <v>0</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="D111" s="23" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E111" s="34" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="F111" s="34">
         <v>8</v>
@@ -8886,13 +8889,13 @@
         <v>0</v>
       </c>
       <c r="C112" s="44" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="D112" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E112" s="45" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="F112" s="45">
         <v>8</v>
@@ -8921,7 +8924,7 @@
         <v>0</v>
       </c>
       <c r="V112" s="47" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="W112" s="44"/>
       <c r="X112" s="43"/>
@@ -8948,13 +8951,13 @@
         <v>0</v>
       </c>
       <c r="C113" s="44" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="D113" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E113" s="45" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="F113" s="45">
         <v>8</v>
@@ -8983,7 +8986,7 @@
         <v>0</v>
       </c>
       <c r="V113" s="47" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="W113" s="44"/>
       <c r="X113" s="43"/>
@@ -9010,10 +9013,10 @@
         <v>0</v>
       </c>
       <c r="C114" s="44" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="D114" s="44" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="E114" s="45" t="s">
         <v>48</v>
@@ -9045,7 +9048,7 @@
         <v>0</v>
       </c>
       <c r="V114" s="47" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="W114" s="44"/>
       <c r="X114" s="43"/>
@@ -9120,7 +9123,7 @@
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
@@ -9146,13 +9149,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
       <c r="F4" s="53" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="G4" s="53"/>
       <c r="H4" s="53"/>
@@ -9167,49 +9170,49 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="H5" s="42" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="J5" s="42" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="N5" s="42" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="O5" s="42" t="s">
         <v>10</v>
       </c>
       <c r="P5" s="42" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -9278,7 +9281,7 @@
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="F9" s="54" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="G9" s="55"/>
       <c r="H9" s="55"/>
@@ -9296,7 +9299,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F10" s="60" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
@@ -9305,7 +9308,7 @@
       <c r="K10" s="55"/>
       <c r="L10" s="55"/>
       <c r="M10" s="58" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="N10" s="58"/>
       <c r="O10" s="59"/>
@@ -9315,7 +9318,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F11" s="57" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="G11" s="55"/>
       <c r="H11" s="55"/>
@@ -9363,69 +9366,69 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B3" s="61"/>
       <c r="C3" s="61"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -9456,7 +9459,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="15" t="s">
@@ -9489,7 +9492,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -9505,13 +9508,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -9527,12 +9530,12 @@
         <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="E9" s="1">
         <v>10</v>
@@ -9540,7 +9543,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>177</v>
@@ -9559,7 +9562,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -9572,7 +9575,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -9582,7 +9585,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" s="38" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to both Excel Data files changes for Line Pattern Also added test servers to the Template data file for example of placing three shapes on the diagram
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D9E2D9-3881-4155-A089-411EC8F5D033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CB03B4-57D1-4555-B967-17AD8A51FFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28125" yWindow="0" windowWidth="27375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="27375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
     <author>Doug Vidakovich</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{CD05495E-E614-47A1-9C25-12C6287B1813}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{77C6CD6B-D70E-4A3B-92C8-21036EFEE591}">
       <text>
         <r>
           <rPr>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="309">
   <si>
     <t>Shape</t>
   </si>
@@ -804,7 +804,52 @@
     <t>Connect From</t>
   </si>
   <si>
+    <t>From LineLabel</t>
+  </si>
+  <si>
+    <t>From LinePattern</t>
+  </si>
+  <si>
+    <t>From ArrowType</t>
+  </si>
+  <si>
+    <t>From LineColor</t>
+  </si>
+  <si>
     <t>Connect To</t>
+  </si>
+  <si>
+    <t>To LineLabel</t>
+  </si>
+  <si>
+    <t>To LinePattern</t>
+  </si>
+  <si>
+    <t>To ArrowType</t>
+  </si>
+  <si>
+    <t>To LineColor</t>
+  </si>
+  <si>
+    <t>mach name</t>
+  </si>
+  <si>
+    <t>mach id</t>
+  </si>
+  <si>
+    <t>site id</t>
+  </si>
+  <si>
+    <t>site name</t>
+  </si>
+  <si>
+    <t>site address</t>
+  </si>
+  <si>
+    <t>omnis name</t>
+  </si>
+  <si>
+    <t>omnis id</t>
   </si>
   <si>
     <t>site_id omnis_id</t>
@@ -1122,58 +1167,10 @@
     <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
   </si>
   <si>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
+  </si>
+  <si>
     <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Advocate_CustomStencils.vssx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
-  </si>
-  <si>
-    <t>Shape Label Font Size</t>
-  </si>
-  <si>
-    <t>From Line Label</t>
-  </si>
-  <si>
-    <t>From Line Pattern</t>
-  </si>
-  <si>
-    <t>From Arrow Type</t>
-  </si>
-  <si>
-    <t>From Line Color</t>
-  </si>
-  <si>
-    <t>To Line Label</t>
-  </si>
-  <si>
-    <t>To Line Pattern</t>
-  </si>
-  <si>
-    <t>To Arrow Type</t>
-  </si>
-  <si>
-    <t>To Line Color</t>
-  </si>
-  <si>
-    <t>mach_name</t>
-  </si>
-  <si>
-    <t>mach_id</t>
-  </si>
-  <si>
-    <t>site_id</t>
-  </si>
-  <si>
-    <t>site_name</t>
-  </si>
-  <si>
-    <t>site_address</t>
-  </si>
-  <si>
-    <t>omnis_name</t>
-  </si>
-  <si>
-    <t>omnis_id</t>
   </si>
   <si>
     <t>Line Pattern</t>
@@ -1582,7 +1579,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1713,6 +1710,15 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1803,7 +1809,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1929,33 +1935,32 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2314,9 +2319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y46" sqref="Y46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y92" sqref="Y92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,8 +2338,8 @@
     <col min="11" max="11" width="7.85546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="8.28515625" style="2" customWidth="1"/>
     <col min="13" max="13" width="6.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" style="3" customWidth="1"/>
     <col min="16" max="16" width="7.28515625" style="3" customWidth="1"/>
     <col min="17" max="17" width="9.28515625" style="1" customWidth="1"/>
     <col min="18" max="19" width="9.140625" style="4"/>
@@ -2356,7 +2361,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>181</v>
@@ -2371,31 +2376,31 @@
         <v>184</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>289</v>
+        <v>185</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>298</v>
+        <v>198</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>299</v>
+        <v>199</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>301</v>
+        <v>201</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>302</v>
+        <v>202</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>303</v>
+        <v>203</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>304</v>
+        <v>204</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>17</v>
@@ -2425,36 +2430,36 @@
         <v>188</v>
       </c>
       <c r="X1" s="33" t="s">
-        <v>290</v>
+        <v>189</v>
       </c>
       <c r="Y1" s="33" t="s">
-        <v>291</v>
+        <v>190</v>
       </c>
       <c r="Z1" s="33" t="s">
-        <v>292</v>
+        <v>191</v>
       </c>
       <c r="AA1" s="33" t="s">
-        <v>293</v>
+        <v>192</v>
       </c>
       <c r="AB1" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="AC1" s="34" t="s">
-        <v>294</v>
+        <v>194</v>
       </c>
       <c r="AD1" s="34" t="s">
-        <v>295</v>
+        <v>195</v>
       </c>
       <c r="AE1" s="34" t="s">
-        <v>296</v>
+        <v>196</v>
       </c>
       <c r="AF1" s="34" t="s">
-        <v>297</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -2490,17 +2495,17 @@
     </row>
     <row r="3" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -2529,21 +2534,13 @@
       <c r="V3" s="24"/>
       <c r="W3" s="21"/>
       <c r="X3" s="23"/>
-      <c r="Y3" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z3" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
       <c r="AA3" s="23"/>
       <c r="AB3" s="23"/>
       <c r="AC3" s="23"/>
-      <c r="AD3" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE3" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
       <c r="AF3" s="23"/>
     </row>
     <row r="4" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2551,12 +2548,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
       <c r="E4" s="40" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -2585,21 +2582,13 @@
       <c r="V4" s="24"/>
       <c r="W4" s="21"/>
       <c r="X4" s="23"/>
-      <c r="Y4" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z4" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
       <c r="AA4" s="23"/>
       <c r="AB4" s="23"/>
       <c r="AC4" s="23"/>
-      <c r="AD4" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE4" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
       <c r="AF4" s="23"/>
     </row>
     <row r="5" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2607,14 +2596,14 @@
         <v>0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="D5" s="21"/>
       <c r="E5" s="21" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
@@ -2643,21 +2632,13 @@
       <c r="V5" s="24"/>
       <c r="W5" s="21"/>
       <c r="X5" s="23"/>
-      <c r="Y5" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z5" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
       <c r="AA5" s="23"/>
       <c r="AB5" s="23"/>
       <c r="AC5" s="23"/>
-      <c r="AD5" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE5" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
       <c r="AF5" s="23"/>
     </row>
     <row r="6" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -2665,14 +2646,14 @@
         <v>0</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="D6" s="40"/>
       <c r="E6" s="40" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
@@ -2701,26 +2682,18 @@
       <c r="V6" s="24"/>
       <c r="W6" s="21"/>
       <c r="X6" s="23"/>
-      <c r="Y6" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z6" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
       <c r="AA6" s="23"/>
       <c r="AB6" s="23"/>
       <c r="AC6" s="23"/>
-      <c r="AD6" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE6" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="19"/>
       <c r="AF6" s="23"/>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -2795,21 +2768,13 @@
       <c r="V8" s="24"/>
       <c r="W8" s="21"/>
       <c r="X8" s="23"/>
-      <c r="Y8" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z8" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
       <c r="AA8" s="23"/>
       <c r="AB8" s="23"/>
       <c r="AC8" s="23"/>
-      <c r="AD8" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE8" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
       <c r="AF8" s="23"/>
     </row>
     <row r="9" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -2820,22 +2785,22 @@
         <v>0</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
@@ -2859,21 +2824,13 @@
       <c r="V9" s="24"/>
       <c r="W9" s="21"/>
       <c r="X9" s="23"/>
-      <c r="Y9" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z9" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y9" s="19"/>
+      <c r="Z9" s="19"/>
       <c r="AA9" s="23"/>
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
-      <c r="AD9" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE9" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD9" s="19"/>
+      <c r="AE9" s="19"/>
       <c r="AF9" s="23"/>
     </row>
     <row r="10" spans="1:32" s="25" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2890,7 +2847,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>204</v>
+        <v>219</v>
       </c>
       <c r="F10" s="21">
         <v>9</v>
@@ -2921,21 +2878,13 @@
       <c r="V10" s="21"/>
       <c r="W10" s="21"/>
       <c r="X10" s="23"/>
-      <c r="Y10" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z10" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
       <c r="AA10" s="23"/>
       <c r="AB10" s="23"/>
       <c r="AC10" s="23"/>
-      <c r="AD10" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE10" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD10" s="19"/>
+      <c r="AE10" s="19"/>
       <c r="AF10" s="23"/>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -3017,18 +2966,12 @@
       <c r="V12" s="24"/>
       <c r="W12" s="21"/>
       <c r="X12" s="23"/>
-      <c r="Y12" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z12" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
       <c r="AA12" s="23"/>
       <c r="AB12" s="21"/>
       <c r="AC12" s="23"/>
-      <c r="AD12" s="19" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD12" s="19"/>
       <c r="AE12" s="19"/>
       <c r="AF12" s="23"/>
     </row>
@@ -3073,23 +3016,19 @@
         <v>0</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="W13" s="21"/>
       <c r="X13" s="23"/>
-      <c r="Y13" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z13" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
       <c r="AA13" s="23"/>
       <c r="AB13" s="21" t="s">
         <v>99</v>
       </c>
       <c r="AC13" s="23"/>
       <c r="AD13" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE13" s="19" t="s">
         <v>27</v>
@@ -3139,23 +3078,19 @@
         <v>0</v>
       </c>
       <c r="V14" s="24" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="W14" s="21"/>
       <c r="X14" s="23"/>
-      <c r="Y14" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z14" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
       <c r="AA14" s="23"/>
       <c r="AB14" s="21" t="s">
         <v>61</v>
       </c>
       <c r="AC14" s="23"/>
       <c r="AD14" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE14" s="19" t="s">
         <v>27</v>
@@ -3205,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="24" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="W15" s="21" t="s">
         <v>58</v>
@@ -3213,8 +3148,8 @@
       <c r="X15" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="Y15" s="23" t="s">
-        <v>307</v>
+      <c r="Y15" s="19" t="s">
+        <v>305</v>
       </c>
       <c r="Z15" s="23" t="s">
         <v>30</v>
@@ -3227,7 +3162,7 @@
       </c>
       <c r="AC15" s="23"/>
       <c r="AD15" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE15" s="19" t="s">
         <v>27</v>
@@ -3277,23 +3212,19 @@
         <v>0</v>
       </c>
       <c r="V16" s="24" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="W16" s="21"/>
       <c r="X16" s="23"/>
-      <c r="Y16" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z16" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
       <c r="AA16" s="23"/>
       <c r="AB16" s="21" t="s">
         <v>61</v>
       </c>
       <c r="AC16" s="23"/>
       <c r="AD16" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE16" s="19" t="s">
         <v>27</v>
@@ -3343,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="W17" s="23" t="s">
         <v>58</v>
@@ -3352,7 +3283,7 @@
         <v>55</v>
       </c>
       <c r="Y17" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z17" s="23" t="s">
         <v>29</v>
@@ -3367,7 +3298,7 @@
         <v>56</v>
       </c>
       <c r="AD17" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE17" s="23" t="s">
         <v>30</v>
@@ -3383,7 +3314,7 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -3455,21 +3386,13 @@
       <c r="V19" s="20"/>
       <c r="W19" s="17"/>
       <c r="X19" s="19"/>
-      <c r="Y19" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z19" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="19"/>
       <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
-      <c r="AD19" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE19" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD19" s="19"/>
+      <c r="AE19" s="19"/>
       <c r="AF19" s="19"/>
     </row>
     <row r="20" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3517,21 +3440,13 @@
       </c>
       <c r="W20" s="17"/>
       <c r="X20" s="19"/>
-      <c r="Y20" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z20" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="19"/>
       <c r="AA20" s="19"/>
       <c r="AB20" s="19"/>
       <c r="AC20" s="19"/>
-      <c r="AD20" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE20" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD20" s="19"/>
+      <c r="AE20" s="19"/>
       <c r="AF20" s="19"/>
     </row>
     <row r="21" spans="1:32" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3579,21 +3494,13 @@
       </c>
       <c r="W21" s="17"/>
       <c r="X21" s="19"/>
-      <c r="Y21" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z21" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y21" s="19"/>
+      <c r="Z21" s="19"/>
       <c r="AA21" s="19"/>
       <c r="AB21" s="19"/>
       <c r="AC21" s="19"/>
-      <c r="AD21" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE21" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD21" s="19"/>
+      <c r="AE21" s="19"/>
       <c r="AF21" s="19"/>
     </row>
     <row r="22" spans="1:32" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3641,21 +3548,13 @@
       </c>
       <c r="W22" s="17"/>
       <c r="X22" s="19"/>
-      <c r="Y22" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z22" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
       <c r="AA22" s="19"/>
       <c r="AB22" s="19"/>
       <c r="AC22" s="19"/>
-      <c r="AD22" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE22" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
       <c r="AF22" s="19"/>
     </row>
     <row r="23" spans="1:32" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3703,21 +3602,13 @@
       </c>
       <c r="W23" s="17"/>
       <c r="X23" s="19"/>
-      <c r="Y23" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z23" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y23" s="19"/>
+      <c r="Z23" s="19"/>
       <c r="AA23" s="19"/>
       <c r="AB23" s="19"/>
       <c r="AC23" s="19"/>
-      <c r="AD23" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE23" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD23" s="19"/>
+      <c r="AE23" s="19"/>
       <c r="AF23" s="19"/>
     </row>
     <row r="24" spans="1:32" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3765,21 +3656,13 @@
       </c>
       <c r="W24" s="17"/>
       <c r="X24" s="19"/>
-      <c r="Y24" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z24" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y24" s="19"/>
+      <c r="Z24" s="19"/>
       <c r="AA24" s="19"/>
       <c r="AB24" s="19"/>
       <c r="AC24" s="19"/>
-      <c r="AD24" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE24" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD24" s="19"/>
+      <c r="AE24" s="19"/>
       <c r="AF24" s="19"/>
     </row>
     <row r="25" spans="1:32" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -3796,7 +3679,7 @@
         <v>34</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -3827,21 +3710,13 @@
       </c>
       <c r="W25" s="17"/>
       <c r="X25" s="19"/>
-      <c r="Y25" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z25" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
       <c r="AA25" s="19"/>
       <c r="AB25" s="19"/>
       <c r="AC25" s="19"/>
-      <c r="AD25" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE25" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
       <c r="AF25" s="19"/>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
@@ -3851,7 +3726,7 @@
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -3874,9 +3749,7 @@
       <c r="W26" s="10"/>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
-      <c r="Z26" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="Z26" s="12"/>
       <c r="AA26" s="12"/>
       <c r="AB26" s="12"/>
       <c r="AC26" s="12"/>
@@ -3898,7 +3771,7 @@
         <v>40</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -3927,21 +3800,13 @@
       <c r="V27" s="24"/>
       <c r="W27" s="21"/>
       <c r="X27" s="23"/>
-      <c r="Y27" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z27" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y27" s="19"/>
+      <c r="Z27" s="19"/>
       <c r="AA27" s="23"/>
       <c r="AB27" s="23"/>
       <c r="AC27" s="23"/>
-      <c r="AD27" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE27" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD27" s="19"/>
+      <c r="AE27" s="19"/>
       <c r="AF27" s="23"/>
     </row>
     <row r="28" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -3985,21 +3850,13 @@
       <c r="V28" s="24"/>
       <c r="W28" s="21"/>
       <c r="X28" s="23"/>
-      <c r="Y28" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z28" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y28" s="19"/>
+      <c r="Z28" s="19"/>
       <c r="AA28" s="23"/>
       <c r="AB28" s="23"/>
       <c r="AC28" s="23"/>
-      <c r="AD28" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE28" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="19"/>
       <c r="AF28" s="23"/>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
@@ -4030,9 +3887,7 @@
       <c r="W29" s="10"/>
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
-      <c r="Z29" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="Z29" s="12"/>
       <c r="AA29" s="12"/>
       <c r="AB29" s="12"/>
       <c r="AC29" s="12"/>
@@ -4090,7 +3945,7 @@
       </c>
       <c r="X30" s="23"/>
       <c r="Y30" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z30" s="23" t="s">
         <v>27</v>
@@ -4105,7 +3960,7 @@
         <v>53</v>
       </c>
       <c r="AD30" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE30" s="23" t="s">
         <v>30</v>
@@ -4164,7 +4019,7 @@
       </c>
       <c r="X31" s="23"/>
       <c r="Y31" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z31" s="23" t="s">
         <v>27</v>
@@ -4174,12 +4029,8 @@
       </c>
       <c r="AB31" s="23"/>
       <c r="AC31" s="23"/>
-      <c r="AD31" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE31" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD31" s="19"/>
+      <c r="AE31" s="19"/>
       <c r="AF31" s="23"/>
     </row>
     <row r="32" spans="1:32" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -4190,13 +4041,13 @@
         <v>0</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>207</v>
+        <v>222</v>
       </c>
       <c r="D32" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>206</v>
+        <v>221</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>177</v>
@@ -4227,21 +4078,13 @@
       <c r="V32" s="24"/>
       <c r="W32" s="21"/>
       <c r="X32" s="23"/>
-      <c r="Y32" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z32" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
       <c r="AA32" s="23"/>
       <c r="AB32" s="23"/>
       <c r="AC32" s="23"/>
-      <c r="AD32" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE32" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD32" s="19"/>
+      <c r="AE32" s="19"/>
       <c r="AF32" s="23"/>
     </row>
     <row r="33" spans="1:32" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4294,7 +4137,7 @@
         <v>89</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>195</v>
+        <v>210</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>177</v>
@@ -4325,21 +4168,13 @@
       <c r="V34" s="24"/>
       <c r="W34" s="21"/>
       <c r="X34" s="23"/>
-      <c r="Y34" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z34" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
       <c r="AA34" s="23"/>
       <c r="AB34" s="23"/>
       <c r="AC34" s="23"/>
-      <c r="AD34" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE34" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="19"/>
       <c r="AF34" s="23"/>
     </row>
     <row r="35" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4392,7 +4227,7 @@
       </c>
       <c r="X35" s="23"/>
       <c r="Y35" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z35" s="23" t="s">
         <v>27</v>
@@ -4402,12 +4237,8 @@
       </c>
       <c r="AB35" s="23"/>
       <c r="AC35" s="23"/>
-      <c r="AD35" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE35" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD35" s="19"/>
+      <c r="AE35" s="19"/>
       <c r="AF35" s="23"/>
     </row>
     <row r="36" spans="1:32" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -4424,7 +4255,7 @@
         <v>18</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
@@ -4453,19 +4284,15 @@
       <c r="V36" s="24"/>
       <c r="W36" s="21"/>
       <c r="X36" s="23"/>
-      <c r="Y36" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z36" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="19"/>
       <c r="AA36" s="23"/>
       <c r="AB36" s="21" t="s">
         <v>81</v>
       </c>
       <c r="AC36" s="23"/>
       <c r="AD36" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE36" s="23" t="s">
         <v>27</v>
@@ -4488,7 +4315,7 @@
         <v>18</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
@@ -4517,19 +4344,15 @@
       <c r="V37" s="24"/>
       <c r="W37" s="21"/>
       <c r="X37" s="23"/>
-      <c r="Y37" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z37" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y37" s="19"/>
+      <c r="Z37" s="19"/>
       <c r="AA37" s="23"/>
       <c r="AB37" s="21" t="s">
         <v>81</v>
       </c>
       <c r="AC37" s="23"/>
       <c r="AD37" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE37" s="23" t="s">
         <v>27</v>
@@ -4588,7 +4411,7 @@
       </c>
       <c r="X38" s="23"/>
       <c r="Y38" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z38" s="23" t="s">
         <v>27</v>
@@ -4601,7 +4424,7 @@
       </c>
       <c r="AC38" s="23"/>
       <c r="AD38" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE38" s="23" t="s">
         <v>27</v>
@@ -4651,19 +4474,15 @@
       <c r="V39" s="24"/>
       <c r="W39" s="21"/>
       <c r="X39" s="23"/>
-      <c r="Y39" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z39" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
       <c r="AA39" s="23"/>
       <c r="AB39" s="23" t="s">
         <v>84</v>
       </c>
       <c r="AC39" s="23"/>
       <c r="AD39" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE39" s="23" t="s">
         <v>27</v>
@@ -4716,13 +4535,13 @@
         <v>0</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="F41" s="21" t="s">
         <v>177</v>
@@ -4753,21 +4572,13 @@
       <c r="V41" s="24"/>
       <c r="W41" s="21"/>
       <c r="X41" s="23"/>
-      <c r="Y41" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z41" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y41" s="19"/>
+      <c r="Z41" s="19"/>
       <c r="AA41" s="23"/>
       <c r="AB41" s="23"/>
       <c r="AC41" s="23"/>
-      <c r="AD41" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE41" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD41" s="19"/>
+      <c r="AE41" s="19"/>
       <c r="AF41" s="23"/>
     </row>
     <row r="42" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4784,7 +4595,7 @@
         <v>50</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
@@ -4820,7 +4631,7 @@
       </c>
       <c r="X42" s="23"/>
       <c r="Y42" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z42" s="23" t="s">
         <v>27</v>
@@ -4830,12 +4641,8 @@
       </c>
       <c r="AB42" s="23"/>
       <c r="AC42" s="23"/>
-      <c r="AD42" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE42" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD42" s="19"/>
+      <c r="AE42" s="19"/>
       <c r="AF42" s="23"/>
     </row>
     <row r="43" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4852,7 +4659,7 @@
         <v>50</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -4888,7 +4695,7 @@
       </c>
       <c r="X43" s="23"/>
       <c r="Y43" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Z43" s="23" t="s">
         <v>27</v>
@@ -4901,7 +4708,7 @@
       </c>
       <c r="AC43" s="23"/>
       <c r="AD43" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE43" s="23" t="s">
         <v>27</v>
@@ -4953,19 +4760,15 @@
       <c r="V44" s="24"/>
       <c r="W44" s="21"/>
       <c r="X44" s="23"/>
-      <c r="Y44" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z44" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y44" s="19"/>
+      <c r="Z44" s="19"/>
       <c r="AA44" s="23"/>
       <c r="AB44" s="23" t="s">
         <v>86</v>
       </c>
       <c r="AC44" s="23"/>
       <c r="AD44" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE44" s="23" t="s">
         <v>27</v>
@@ -5051,21 +4854,13 @@
       <c r="V46" s="24"/>
       <c r="W46" s="21"/>
       <c r="X46" s="23"/>
-      <c r="Y46" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z46" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y46" s="19"/>
+      <c r="Z46" s="19"/>
       <c r="AA46" s="23"/>
       <c r="AB46" s="23"/>
       <c r="AC46" s="23"/>
-      <c r="AD46" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE46" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD46" s="19"/>
+      <c r="AE46" s="19"/>
       <c r="AF46" s="23"/>
     </row>
     <row r="47" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -5082,7 +4877,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
@@ -5111,21 +4906,13 @@
       <c r="V47" s="24"/>
       <c r="W47" s="21"/>
       <c r="X47" s="23"/>
-      <c r="Y47" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z47" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y47" s="19"/>
+      <c r="Z47" s="19"/>
       <c r="AA47" s="23"/>
       <c r="AB47" s="23"/>
       <c r="AC47" s="23"/>
-      <c r="AD47" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE47" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD47" s="19"/>
+      <c r="AE47" s="19"/>
       <c r="AF47" s="23"/>
     </row>
     <row r="48" spans="1:32" s="25" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5142,7 +4929,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="F48" s="32">
         <v>10</v>
@@ -5173,21 +4960,13 @@
       <c r="V48" s="21"/>
       <c r="W48" s="21"/>
       <c r="X48" s="23"/>
-      <c r="Y48" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z48" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y48" s="19"/>
+      <c r="Z48" s="19"/>
       <c r="AA48" s="23"/>
       <c r="AB48" s="23"/>
       <c r="AC48" s="23"/>
-      <c r="AD48" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE48" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD48" s="19"/>
+      <c r="AE48" s="19"/>
       <c r="AF48" s="23"/>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.25">
@@ -5269,21 +5048,13 @@
       <c r="V50" s="24"/>
       <c r="W50" s="21"/>
       <c r="X50" s="23"/>
-      <c r="Y50" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z50" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y50" s="19"/>
+      <c r="Z50" s="19"/>
       <c r="AA50" s="23"/>
       <c r="AB50" s="23"/>
       <c r="AC50" s="23"/>
-      <c r="AD50" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE50" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD50" s="19"/>
+      <c r="AE50" s="19"/>
       <c r="AF50" s="23"/>
     </row>
     <row r="51" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -5300,7 +5071,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="F51" s="21"/>
       <c r="G51" s="21"/>
@@ -5329,21 +5100,13 @@
       <c r="V51" s="24"/>
       <c r="W51" s="21"/>
       <c r="X51" s="23"/>
-      <c r="Y51" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z51" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y51" s="19"/>
+      <c r="Z51" s="19"/>
       <c r="AA51" s="23"/>
       <c r="AB51" s="23"/>
       <c r="AC51" s="23"/>
-      <c r="AD51" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE51" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD51" s="19"/>
+      <c r="AE51" s="19"/>
       <c r="AF51" s="23"/>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.25">
@@ -5425,19 +5188,15 @@
       <c r="V53" s="20"/>
       <c r="W53" s="17"/>
       <c r="X53" s="19"/>
-      <c r="Y53" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z53" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA53" s="19"/>
+      <c r="Y53" s="19"/>
+      <c r="Z53" s="19"/>
+      <c r="AA53" s="23"/>
       <c r="AB53" s="17" t="s">
         <v>76</v>
       </c>
       <c r="AC53" s="19"/>
       <c r="AD53" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE53" s="19" t="s">
         <v>28</v>
@@ -5487,19 +5246,15 @@
       <c r="V54" s="20"/>
       <c r="W54" s="17"/>
       <c r="X54" s="19"/>
-      <c r="Y54" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z54" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA54" s="19"/>
+      <c r="Y54" s="19"/>
+      <c r="Z54" s="19"/>
+      <c r="AA54" s="23"/>
       <c r="AB54" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC54" s="19"/>
       <c r="AD54" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE54" s="19" t="s">
         <v>28</v>
@@ -5549,19 +5304,15 @@
       <c r="V55" s="30"/>
       <c r="W55" s="28"/>
       <c r="X55" s="27"/>
-      <c r="Y55" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z55" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y55" s="27"/>
+      <c r="Z55" s="27"/>
       <c r="AA55" s="27"/>
       <c r="AB55" s="28" t="s">
         <v>78</v>
       </c>
       <c r="AC55" s="27"/>
-      <c r="AD55" s="60" t="s">
-        <v>306</v>
+      <c r="AD55" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE55" s="27" t="s">
         <v>28</v>
@@ -5611,19 +5362,15 @@
       <c r="V56" s="30"/>
       <c r="W56" s="28"/>
       <c r="X56" s="27"/>
-      <c r="Y56" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z56" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y56" s="27"/>
+      <c r="Z56" s="27"/>
       <c r="AA56" s="27"/>
       <c r="AB56" s="28" t="s">
         <v>105</v>
       </c>
       <c r="AC56" s="27"/>
-      <c r="AD56" s="60" t="s">
-        <v>306</v>
+      <c r="AD56" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE56" s="27" t="s">
         <v>28</v>
@@ -5673,19 +5420,15 @@
       <c r="V57" s="20"/>
       <c r="W57" s="17"/>
       <c r="X57" s="19"/>
-      <c r="Y57" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z57" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA57" s="19"/>
+      <c r="Y57" s="19"/>
+      <c r="Z57" s="19"/>
+      <c r="AA57" s="23"/>
       <c r="AB57" s="17" t="s">
         <v>74</v>
       </c>
       <c r="AC57" s="19"/>
       <c r="AD57" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE57" s="19" t="s">
         <v>28</v>
@@ -5735,19 +5478,15 @@
       <c r="V58" s="20"/>
       <c r="W58" s="17"/>
       <c r="X58" s="19"/>
-      <c r="Y58" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z58" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA58" s="19"/>
+      <c r="Y58" s="19"/>
+      <c r="Z58" s="19"/>
+      <c r="AA58" s="23"/>
       <c r="AB58" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC58" s="19"/>
       <c r="AD58" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE58" s="19" t="s">
         <v>28</v>
@@ -5797,19 +5536,15 @@
       <c r="V59" s="30"/>
       <c r="W59" s="28"/>
       <c r="X59" s="27"/>
-      <c r="Y59" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z59" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y59" s="27"/>
+      <c r="Z59" s="27"/>
       <c r="AA59" s="27"/>
       <c r="AB59" s="28" t="s">
         <v>110</v>
       </c>
       <c r="AC59" s="27"/>
-      <c r="AD59" s="60" t="s">
-        <v>306</v>
+      <c r="AD59" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE59" s="27" t="s">
         <v>28</v>
@@ -5859,19 +5594,15 @@
       <c r="V60" s="30"/>
       <c r="W60" s="28"/>
       <c r="X60" s="27"/>
-      <c r="Y60" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z60" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y60" s="27"/>
+      <c r="Z60" s="27"/>
       <c r="AA60" s="27"/>
       <c r="AB60" s="28" t="s">
         <v>105</v>
       </c>
       <c r="AC60" s="27"/>
-      <c r="AD60" s="60" t="s">
-        <v>306</v>
+      <c r="AD60" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE60" s="27" t="s">
         <v>28</v>
@@ -5921,19 +5652,15 @@
       <c r="V61" s="20"/>
       <c r="W61" s="17"/>
       <c r="X61" s="19"/>
-      <c r="Y61" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z61" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA61" s="19"/>
+      <c r="Y61" s="19"/>
+      <c r="Z61" s="19"/>
+      <c r="AA61" s="23"/>
       <c r="AB61" s="17" t="s">
         <v>111</v>
       </c>
       <c r="AC61" s="19"/>
       <c r="AD61" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE61" s="19" t="s">
         <v>28</v>
@@ -5983,19 +5710,15 @@
       <c r="V62" s="20"/>
       <c r="W62" s="17"/>
       <c r="X62" s="19"/>
-      <c r="Y62" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z62" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA62" s="19"/>
+      <c r="Y62" s="19"/>
+      <c r="Z62" s="19"/>
+      <c r="AA62" s="23"/>
       <c r="AB62" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC62" s="19"/>
       <c r="AD62" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE62" s="19" t="s">
         <v>28</v>
@@ -6045,19 +5768,15 @@
       <c r="V63" s="30"/>
       <c r="W63" s="28"/>
       <c r="X63" s="27"/>
-      <c r="Y63" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z63" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y63" s="27"/>
+      <c r="Z63" s="27"/>
       <c r="AA63" s="27"/>
       <c r="AB63" s="28" t="s">
         <v>108</v>
       </c>
       <c r="AC63" s="27"/>
-      <c r="AD63" s="60" t="s">
-        <v>306</v>
+      <c r="AD63" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE63" s="27" t="s">
         <v>28</v>
@@ -6107,19 +5826,15 @@
       <c r="V64" s="30"/>
       <c r="W64" s="28"/>
       <c r="X64" s="27"/>
-      <c r="Y64" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z64" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y64" s="27"/>
+      <c r="Z64" s="27"/>
       <c r="AA64" s="27"/>
       <c r="AB64" s="28" t="s">
         <v>105</v>
       </c>
       <c r="AC64" s="27"/>
-      <c r="AD64" s="60" t="s">
-        <v>306</v>
+      <c r="AD64" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE64" s="27" t="s">
         <v>28</v>
@@ -6140,7 +5855,7 @@
         <v>7</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
@@ -6169,19 +5884,15 @@
       <c r="V65" s="20"/>
       <c r="W65" s="17"/>
       <c r="X65" s="19"/>
-      <c r="Y65" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z65" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA65" s="19"/>
+      <c r="Y65" s="19"/>
+      <c r="Z65" s="19"/>
+      <c r="AA65" s="23"/>
       <c r="AB65" s="17" t="s">
         <v>109</v>
       </c>
       <c r="AC65" s="19"/>
       <c r="AD65" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE65" s="19" t="s">
         <v>28</v>
@@ -6204,7 +5915,7 @@
         <v>10</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="17"/>
@@ -6233,19 +5944,15 @@
       <c r="V66" s="20"/>
       <c r="W66" s="17"/>
       <c r="X66" s="19"/>
-      <c r="Y66" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z66" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA66" s="19"/>
+      <c r="Y66" s="19"/>
+      <c r="Z66" s="19"/>
+      <c r="AA66" s="23"/>
       <c r="AB66" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC66" s="19"/>
       <c r="AD66" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE66" s="19" t="s">
         <v>28</v>
@@ -6262,13 +5969,13 @@
         <v>0</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="D67" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="F67" s="21"/>
       <c r="G67" s="21"/>
@@ -6299,21 +6006,13 @@
       </c>
       <c r="W67" s="21"/>
       <c r="X67" s="23"/>
-      <c r="Y67" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z67" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y67" s="19"/>
+      <c r="Z67" s="19"/>
       <c r="AA67" s="23"/>
       <c r="AB67" s="23"/>
       <c r="AC67" s="23"/>
-      <c r="AD67" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE67" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD67" s="19"/>
+      <c r="AE67" s="23"/>
       <c r="AF67" s="23"/>
     </row>
     <row r="68" spans="1:32" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -6359,19 +6058,15 @@
       <c r="V68" s="30"/>
       <c r="W68" s="28"/>
       <c r="X68" s="27"/>
-      <c r="Y68" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z68" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y68" s="27"/>
+      <c r="Z68" s="27"/>
       <c r="AA68" s="27"/>
       <c r="AB68" s="28" t="s">
         <v>112</v>
       </c>
       <c r="AC68" s="27"/>
-      <c r="AD68" s="60" t="s">
-        <v>306</v>
+      <c r="AD68" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE68" s="27" t="s">
         <v>28</v>
@@ -6421,19 +6116,15 @@
       <c r="V69" s="30"/>
       <c r="W69" s="28"/>
       <c r="X69" s="27"/>
-      <c r="Y69" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z69" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y69" s="27"/>
+      <c r="Z69" s="27"/>
       <c r="AA69" s="27"/>
       <c r="AB69" s="28" t="s">
         <v>105</v>
       </c>
       <c r="AC69" s="27"/>
-      <c r="AD69" s="60" t="s">
-        <v>306</v>
+      <c r="AD69" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE69" s="27" t="s">
         <v>28</v>
@@ -6483,19 +6174,15 @@
       <c r="V70" s="20"/>
       <c r="W70" s="17"/>
       <c r="X70" s="19"/>
-      <c r="Y70" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z70" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA70" s="19"/>
+      <c r="Y70" s="19"/>
+      <c r="Z70" s="19"/>
+      <c r="AA70" s="23"/>
       <c r="AB70" s="17" t="s">
         <v>113</v>
       </c>
       <c r="AC70" s="19"/>
       <c r="AD70" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE70" s="19" t="s">
         <v>28</v>
@@ -6545,19 +6232,15 @@
       <c r="V71" s="20"/>
       <c r="W71" s="17"/>
       <c r="X71" s="19"/>
-      <c r="Y71" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z71" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA71" s="19"/>
+      <c r="Y71" s="19"/>
+      <c r="Z71" s="19"/>
+      <c r="AA71" s="23"/>
       <c r="AB71" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC71" s="19"/>
       <c r="AD71" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE71" s="19" t="s">
         <v>28</v>
@@ -6607,19 +6290,15 @@
       <c r="V72" s="30"/>
       <c r="W72" s="28"/>
       <c r="X72" s="27"/>
-      <c r="Y72" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z72" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y72" s="27"/>
+      <c r="Z72" s="27"/>
       <c r="AA72" s="27"/>
       <c r="AB72" s="27" t="s">
         <v>135</v>
       </c>
       <c r="AC72" s="27"/>
-      <c r="AD72" s="60" t="s">
-        <v>306</v>
+      <c r="AD72" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE72" s="27" t="s">
         <v>27</v>
@@ -6654,9 +6333,7 @@
       <c r="W73" s="10"/>
       <c r="X73" s="12"/>
       <c r="Y73" s="12"/>
-      <c r="Z73" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="Z73" s="12"/>
       <c r="AA73" s="12"/>
       <c r="AB73" s="12"/>
       <c r="AC73" s="12"/>
@@ -6707,19 +6384,15 @@
       <c r="V74" s="20"/>
       <c r="W74" s="17"/>
       <c r="X74" s="19"/>
-      <c r="Y74" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z74" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA74" s="19"/>
+      <c r="Y74" s="19"/>
+      <c r="Z74" s="19"/>
+      <c r="AA74" s="23"/>
       <c r="AB74" s="17" t="s">
         <v>105</v>
       </c>
       <c r="AC74" s="19"/>
       <c r="AD74" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE74" s="19" t="s">
         <v>28</v>
@@ -6769,19 +6442,15 @@
       <c r="V75" s="20"/>
       <c r="W75" s="17"/>
       <c r="X75" s="19"/>
-      <c r="Y75" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z75" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA75" s="19"/>
+      <c r="Y75" s="19"/>
+      <c r="Z75" s="19"/>
+      <c r="AA75" s="23"/>
       <c r="AB75" s="17" t="s">
         <v>163</v>
       </c>
       <c r="AC75" s="19"/>
       <c r="AD75" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE75" s="19" t="s">
         <v>28</v>
@@ -6867,21 +6536,13 @@
       <c r="V77" s="24"/>
       <c r="W77" s="21"/>
       <c r="X77" s="23"/>
-      <c r="Y77" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z77" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y77" s="19"/>
+      <c r="Z77" s="19"/>
       <c r="AA77" s="23"/>
       <c r="AB77" s="23"/>
       <c r="AC77" s="23"/>
-      <c r="AD77" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE77" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD77" s="19"/>
+      <c r="AE77" s="19"/>
       <c r="AF77" s="23"/>
     </row>
     <row r="78" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -6925,21 +6586,13 @@
       <c r="V78" s="24"/>
       <c r="W78" s="21"/>
       <c r="X78" s="23"/>
-      <c r="Y78" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z78" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y78" s="19"/>
+      <c r="Z78" s="19"/>
       <c r="AA78" s="23"/>
       <c r="AB78" s="23"/>
       <c r="AC78" s="23"/>
-      <c r="AD78" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE78" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD78" s="19"/>
+      <c r="AE78" s="19"/>
       <c r="AF78" s="23"/>
     </row>
     <row r="79" spans="1:32" x14ac:dyDescent="0.25">
@@ -7021,19 +6674,15 @@
       <c r="V80" s="20"/>
       <c r="W80" s="17"/>
       <c r="X80" s="19"/>
-      <c r="Y80" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z80" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA80" s="19"/>
+      <c r="Y80" s="19"/>
+      <c r="Z80" s="19"/>
+      <c r="AA80" s="23"/>
       <c r="AB80" s="17" t="s">
         <v>138</v>
       </c>
       <c r="AC80" s="19"/>
       <c r="AD80" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE80" s="19" t="s">
         <v>28</v>
@@ -7083,19 +6732,15 @@
       <c r="V81" s="20"/>
       <c r="W81" s="17"/>
       <c r="X81" s="19"/>
-      <c r="Y81" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z81" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA81" s="19"/>
+      <c r="Y81" s="19"/>
+      <c r="Z81" s="19"/>
+      <c r="AA81" s="23"/>
       <c r="AB81" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC81" s="19"/>
       <c r="AD81" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE81" s="19" t="s">
         <v>28</v>
@@ -7145,19 +6790,15 @@
       <c r="V82" s="30"/>
       <c r="W82" s="28"/>
       <c r="X82" s="27"/>
-      <c r="Y82" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z82" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y82" s="27"/>
+      <c r="Z82" s="27"/>
       <c r="AA82" s="27"/>
       <c r="AB82" s="28" t="s">
         <v>140</v>
       </c>
       <c r="AC82" s="27"/>
-      <c r="AD82" s="60" t="s">
-        <v>306</v>
+      <c r="AD82" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE82" s="27" t="s">
         <v>28</v>
@@ -7207,19 +6848,15 @@
       <c r="V83" s="30"/>
       <c r="W83" s="28"/>
       <c r="X83" s="27"/>
-      <c r="Y83" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z83" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y83" s="27"/>
+      <c r="Z83" s="27"/>
       <c r="AA83" s="27"/>
       <c r="AB83" s="28" t="s">
         <v>156</v>
       </c>
       <c r="AC83" s="27"/>
-      <c r="AD83" s="60" t="s">
-        <v>306</v>
+      <c r="AD83" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE83" s="27" t="s">
         <v>28</v>
@@ -7269,19 +6906,15 @@
       <c r="V84" s="20"/>
       <c r="W84" s="17"/>
       <c r="X84" s="19"/>
-      <c r="Y84" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z84" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA84" s="19"/>
+      <c r="Y84" s="19"/>
+      <c r="Z84" s="19"/>
+      <c r="AA84" s="23"/>
       <c r="AB84" s="17" t="s">
         <v>142</v>
       </c>
       <c r="AC84" s="19"/>
       <c r="AD84" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE84" s="19" t="s">
         <v>28</v>
@@ -7331,19 +6964,15 @@
       <c r="V85" s="20"/>
       <c r="W85" s="17"/>
       <c r="X85" s="19"/>
-      <c r="Y85" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z85" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA85" s="19"/>
+      <c r="Y85" s="19"/>
+      <c r="Z85" s="19"/>
+      <c r="AA85" s="23"/>
       <c r="AB85" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC85" s="19"/>
       <c r="AD85" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE85" s="19" t="s">
         <v>28</v>
@@ -7393,19 +7022,15 @@
       <c r="V86" s="30"/>
       <c r="W86" s="28"/>
       <c r="X86" s="27"/>
-      <c r="Y86" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z86" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y86" s="27"/>
+      <c r="Z86" s="27"/>
       <c r="AA86" s="27"/>
       <c r="AB86" s="28" t="s">
         <v>144</v>
       </c>
       <c r="AC86" s="27"/>
-      <c r="AD86" s="60" t="s">
-        <v>306</v>
+      <c r="AD86" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE86" s="27" t="s">
         <v>28</v>
@@ -7455,19 +7080,15 @@
       <c r="V87" s="30"/>
       <c r="W87" s="28"/>
       <c r="X87" s="27"/>
-      <c r="Y87" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z87" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y87" s="27"/>
+      <c r="Z87" s="27"/>
       <c r="AA87" s="27"/>
       <c r="AB87" s="28" t="s">
         <v>156</v>
       </c>
       <c r="AC87" s="27"/>
-      <c r="AD87" s="60" t="s">
-        <v>306</v>
+      <c r="AD87" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE87" s="27" t="s">
         <v>28</v>
@@ -7517,19 +7138,15 @@
       <c r="V88" s="20"/>
       <c r="W88" s="17"/>
       <c r="X88" s="19"/>
-      <c r="Y88" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z88" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA88" s="19"/>
+      <c r="Y88" s="19"/>
+      <c r="Z88" s="19"/>
+      <c r="AA88" s="23"/>
       <c r="AB88" s="17" t="s">
         <v>147</v>
       </c>
       <c r="AC88" s="19"/>
       <c r="AD88" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE88" s="19" t="s">
         <v>28</v>
@@ -7579,19 +7196,15 @@
       <c r="V89" s="20"/>
       <c r="W89" s="17"/>
       <c r="X89" s="19"/>
-      <c r="Y89" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z89" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA89" s="19"/>
+      <c r="Y89" s="19"/>
+      <c r="Z89" s="19"/>
+      <c r="AA89" s="23"/>
       <c r="AB89" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC89" s="19"/>
       <c r="AD89" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE89" s="19" t="s">
         <v>28</v>
@@ -7641,19 +7254,15 @@
       <c r="V90" s="30"/>
       <c r="W90" s="28"/>
       <c r="X90" s="27"/>
-      <c r="Y90" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z90" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y90" s="27"/>
+      <c r="Z90" s="27"/>
       <c r="AA90" s="27"/>
       <c r="AB90" s="28" t="s">
         <v>149</v>
       </c>
       <c r="AC90" s="27"/>
-      <c r="AD90" s="60" t="s">
-        <v>306</v>
+      <c r="AD90" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE90" s="27" t="s">
         <v>28</v>
@@ -7703,19 +7312,15 @@
       <c r="V91" s="30"/>
       <c r="W91" s="28"/>
       <c r="X91" s="27"/>
-      <c r="Y91" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z91" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y91" s="27"/>
+      <c r="Z91" s="27"/>
       <c r="AA91" s="27"/>
       <c r="AB91" s="28" t="s">
         <v>156</v>
       </c>
       <c r="AC91" s="27"/>
-      <c r="AD91" s="60" t="s">
-        <v>306</v>
+      <c r="AD91" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE91" s="27" t="s">
         <v>28</v>
@@ -7736,7 +7341,7 @@
         <v>7</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="17"/>
@@ -7765,19 +7370,15 @@
       <c r="V92" s="20"/>
       <c r="W92" s="17"/>
       <c r="X92" s="19"/>
-      <c r="Y92" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z92" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA92" s="19"/>
+      <c r="Y92" s="19"/>
+      <c r="Z92" s="19"/>
+      <c r="AA92" s="23"/>
       <c r="AB92" s="17" t="s">
         <v>151</v>
       </c>
       <c r="AC92" s="19"/>
       <c r="AD92" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE92" s="19" t="s">
         <v>28</v>
@@ -7800,7 +7401,7 @@
         <v>10</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="17"/>
@@ -7829,19 +7430,15 @@
       <c r="V93" s="20"/>
       <c r="W93" s="17"/>
       <c r="X93" s="19"/>
-      <c r="Y93" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z93" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA93" s="19"/>
+      <c r="Y93" s="19"/>
+      <c r="Z93" s="19"/>
+      <c r="AA93" s="23"/>
       <c r="AB93" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC93" s="19"/>
       <c r="AD93" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AE93" s="19" t="s">
         <v>28</v>
@@ -7858,13 +7455,13 @@
         <v>0</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="D94" s="21" t="s">
         <v>89</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="F94" s="21"/>
       <c r="G94" s="21"/>
@@ -7895,21 +7492,13 @@
       </c>
       <c r="W94" s="21"/>
       <c r="X94" s="23"/>
-      <c r="Y94" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z94" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y94" s="19"/>
+      <c r="Z94" s="19"/>
       <c r="AA94" s="23"/>
       <c r="AB94" s="23"/>
       <c r="AC94" s="23"/>
-      <c r="AD94" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE94" s="23" t="s">
-        <v>28</v>
-      </c>
+      <c r="AD94" s="19"/>
+      <c r="AE94" s="23"/>
       <c r="AF94" s="23"/>
     </row>
     <row r="95" spans="1:32" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -7955,19 +7544,15 @@
       <c r="V95" s="30"/>
       <c r="W95" s="28"/>
       <c r="X95" s="27"/>
-      <c r="Y95" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z95" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y95" s="27"/>
+      <c r="Z95" s="27"/>
       <c r="AA95" s="27"/>
       <c r="AB95" s="28" t="s">
         <v>153</v>
       </c>
       <c r="AC95" s="27"/>
-      <c r="AD95" s="60" t="s">
-        <v>306</v>
+      <c r="AD95" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE95" s="27" t="s">
         <v>28</v>
@@ -8017,19 +7602,15 @@
       <c r="V96" s="30"/>
       <c r="W96" s="28"/>
       <c r="X96" s="27"/>
-      <c r="Y96" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z96" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y96" s="27"/>
+      <c r="Z96" s="27"/>
       <c r="AA96" s="27"/>
       <c r="AB96" s="28" t="s">
         <v>156</v>
       </c>
       <c r="AC96" s="27"/>
-      <c r="AD96" s="60" t="s">
-        <v>306</v>
+      <c r="AD96" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE96" s="27" t="s">
         <v>28</v>
@@ -8079,19 +7660,15 @@
       <c r="V97" s="20"/>
       <c r="W97" s="17"/>
       <c r="X97" s="19"/>
-      <c r="Y97" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z97" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA97" s="19"/>
+      <c r="Y97" s="19"/>
+      <c r="Z97" s="19"/>
+      <c r="AA97" s="23"/>
       <c r="AB97" s="17" t="s">
         <v>155</v>
       </c>
       <c r="AC97" s="19"/>
       <c r="AD97" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE97" s="19" t="s">
         <v>28</v>
@@ -8141,19 +7718,15 @@
       <c r="V98" s="20"/>
       <c r="W98" s="17"/>
       <c r="X98" s="19"/>
-      <c r="Y98" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z98" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA98" s="19"/>
+      <c r="Y98" s="19"/>
+      <c r="Z98" s="19"/>
+      <c r="AA98" s="23"/>
       <c r="AB98" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC98" s="19"/>
       <c r="AD98" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE98" s="19" t="s">
         <v>28</v>
@@ -8203,19 +7776,15 @@
       <c r="V99" s="30"/>
       <c r="W99" s="28"/>
       <c r="X99" s="27"/>
-      <c r="Y99" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z99" s="27" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y99" s="27"/>
+      <c r="Z99" s="27"/>
       <c r="AA99" s="27"/>
       <c r="AB99" s="27" t="s">
         <v>135</v>
       </c>
       <c r="AC99" s="27"/>
-      <c r="AD99" s="60" t="s">
-        <v>306</v>
+      <c r="AD99" s="27" t="s">
+        <v>305</v>
       </c>
       <c r="AE99" s="27" t="s">
         <v>27</v>
@@ -8250,9 +7819,7 @@
       <c r="W100" s="10"/>
       <c r="X100" s="12"/>
       <c r="Y100" s="12"/>
-      <c r="Z100" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="Z100" s="12"/>
       <c r="AA100" s="12"/>
       <c r="AB100" s="12"/>
       <c r="AC100" s="12"/>
@@ -8303,19 +7870,15 @@
       <c r="V101" s="20"/>
       <c r="W101" s="17"/>
       <c r="X101" s="19"/>
-      <c r="Y101" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z101" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA101" s="19"/>
+      <c r="Y101" s="19"/>
+      <c r="Z101" s="19"/>
+      <c r="AA101" s="23"/>
       <c r="AB101" s="17" t="s">
         <v>156</v>
       </c>
       <c r="AC101" s="19"/>
       <c r="AD101" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE101" s="19" t="s">
         <v>28</v>
@@ -8365,19 +7928,15 @@
       <c r="V102" s="20"/>
       <c r="W102" s="17"/>
       <c r="X102" s="19"/>
-      <c r="Y102" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z102" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA102" s="19"/>
+      <c r="Y102" s="19"/>
+      <c r="Z102" s="19"/>
+      <c r="AA102" s="23"/>
       <c r="AB102" s="17" t="s">
         <v>146</v>
       </c>
       <c r="AC102" s="19"/>
       <c r="AD102" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE102" s="19" t="s">
         <v>28</v>
@@ -8412,9 +7971,7 @@
       <c r="W103" s="10"/>
       <c r="X103" s="12"/>
       <c r="Y103" s="12"/>
-      <c r="Z103" s="12" t="s">
-        <v>28</v>
-      </c>
+      <c r="Z103" s="12"/>
       <c r="AA103" s="12"/>
       <c r="AB103" s="12"/>
       <c r="AC103" s="12"/>
@@ -8467,19 +8024,15 @@
       <c r="V104" s="24"/>
       <c r="W104" s="21"/>
       <c r="X104" s="23"/>
-      <c r="Y104" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z104" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y104" s="19"/>
+      <c r="Z104" s="19"/>
       <c r="AA104" s="23"/>
       <c r="AB104" s="19" t="s">
         <v>135</v>
       </c>
       <c r="AC104" s="23"/>
       <c r="AD104" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AE104" s="19" t="s">
         <v>27</v>
@@ -8490,7 +8043,7 @@
     </row>
     <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="B105" s="10"/>
       <c r="C105" s="10"/>
@@ -8532,13 +8085,13 @@
         <v>0</v>
       </c>
       <c r="C106" s="40" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="D106" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E106" s="41" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="F106" s="41">
         <v>8</v>
@@ -8571,18 +8124,12 @@
       </c>
       <c r="W106" s="40"/>
       <c r="X106" s="39"/>
-      <c r="Y106" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z106" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y106" s="39"/>
+      <c r="Z106" s="39"/>
       <c r="AA106" s="39"/>
       <c r="AB106" s="39"/>
       <c r="AC106" s="39"/>
-      <c r="AD106" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD106" s="39"/>
       <c r="AE106" s="39"/>
       <c r="AF106" s="39"/>
     </row>
@@ -8594,13 +8141,13 @@
         <v>0</v>
       </c>
       <c r="C107" s="40" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D107" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E107" s="41" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="F107" s="41">
         <v>8</v>
@@ -8633,18 +8180,12 @@
       </c>
       <c r="W107" s="40"/>
       <c r="X107" s="39"/>
-      <c r="Y107" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z107" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y107" s="39"/>
+      <c r="Z107" s="39"/>
       <c r="AA107" s="39"/>
       <c r="AB107" s="39"/>
       <c r="AC107" s="39"/>
-      <c r="AD107" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD107" s="39"/>
       <c r="AE107" s="39"/>
       <c r="AF107" s="39"/>
     </row>
@@ -8656,13 +8197,13 @@
         <v>0</v>
       </c>
       <c r="C108" s="40" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="D108" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E108" s="41" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="F108" s="41">
         <v>8</v>
@@ -8695,18 +8236,12 @@
       </c>
       <c r="W108" s="40"/>
       <c r="X108" s="39"/>
-      <c r="Y108" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z108" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y108" s="39"/>
+      <c r="Z108" s="39"/>
       <c r="AA108" s="39"/>
       <c r="AB108" s="39"/>
       <c r="AC108" s="39"/>
-      <c r="AD108" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD108" s="39"/>
       <c r="AE108" s="39"/>
       <c r="AF108" s="39"/>
     </row>
@@ -8718,13 +8253,13 @@
         <v>0</v>
       </c>
       <c r="C109" s="21" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="D109" s="21" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="F109" s="32">
         <v>8</v>
@@ -8755,18 +8290,12 @@
       <c r="V109" s="24"/>
       <c r="W109" s="21"/>
       <c r="X109" s="23"/>
-      <c r="Y109" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z109" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y109" s="19"/>
+      <c r="Z109" s="19"/>
       <c r="AA109" s="23"/>
       <c r="AB109" s="19"/>
       <c r="AC109" s="23"/>
-      <c r="AD109" s="19" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD109" s="19"/>
       <c r="AE109" s="19"/>
       <c r="AF109" s="23"/>
     </row>
@@ -8778,13 +8307,13 @@
         <v>0</v>
       </c>
       <c r="C110" s="21" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="D110" s="21" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="F110" s="32">
         <v>8</v>
@@ -8815,18 +8344,12 @@
       <c r="V110" s="24"/>
       <c r="W110" s="21"/>
       <c r="X110" s="23"/>
-      <c r="Y110" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z110" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y110" s="19"/>
+      <c r="Z110" s="19"/>
       <c r="AA110" s="23"/>
       <c r="AB110" s="19"/>
       <c r="AC110" s="23"/>
-      <c r="AD110" s="19" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD110" s="19"/>
       <c r="AE110" s="19"/>
       <c r="AF110" s="23"/>
     </row>
@@ -8838,13 +8361,13 @@
         <v>0</v>
       </c>
       <c r="C111" s="21" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E111" s="32" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="F111" s="32">
         <v>8</v>
@@ -8875,18 +8398,12 @@
       <c r="V111" s="24"/>
       <c r="W111" s="21"/>
       <c r="X111" s="23"/>
-      <c r="Y111" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z111" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y111" s="19"/>
+      <c r="Z111" s="19"/>
       <c r="AA111" s="23"/>
       <c r="AB111" s="19"/>
       <c r="AC111" s="23"/>
-      <c r="AD111" s="19" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD111" s="19"/>
       <c r="AE111" s="19"/>
       <c r="AF111" s="23"/>
     </row>
@@ -8898,13 +8415,13 @@
         <v>0</v>
       </c>
       <c r="C112" s="40" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="D112" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E112" s="41" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F112" s="41">
         <v>8</v>
@@ -8933,22 +8450,16 @@
         <v>0</v>
       </c>
       <c r="V112" s="43" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="W112" s="40"/>
       <c r="X112" s="39"/>
-      <c r="Y112" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z112" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y112" s="39"/>
+      <c r="Z112" s="39"/>
       <c r="AA112" s="39"/>
       <c r="AB112" s="39"/>
       <c r="AC112" s="39"/>
-      <c r="AD112" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD112" s="39"/>
       <c r="AE112" s="39"/>
       <c r="AF112" s="39"/>
     </row>
@@ -8960,13 +8471,13 @@
         <v>0</v>
       </c>
       <c r="C113" s="40" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="D113" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E113" s="41" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F113" s="41">
         <v>8</v>
@@ -8995,22 +8506,16 @@
         <v>0</v>
       </c>
       <c r="V113" s="43" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="W113" s="40"/>
       <c r="X113" s="39"/>
-      <c r="Y113" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z113" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y113" s="39"/>
+      <c r="Z113" s="39"/>
       <c r="AA113" s="39"/>
       <c r="AB113" s="39"/>
       <c r="AC113" s="39"/>
-      <c r="AD113" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD113" s="39"/>
       <c r="AE113" s="39"/>
       <c r="AF113" s="39"/>
     </row>
@@ -9022,10 +8527,10 @@
         <v>0</v>
       </c>
       <c r="C114" s="40" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="D114" s="40" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="E114" s="41" t="s">
         <v>48</v>
@@ -9057,22 +8562,16 @@
         <v>0</v>
       </c>
       <c r="V114" s="43" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="W114" s="40"/>
       <c r="X114" s="39"/>
-      <c r="Y114" s="39" t="s">
-        <v>306</v>
-      </c>
-      <c r="Z114" s="39" t="s">
-        <v>28</v>
-      </c>
+      <c r="Y114" s="39"/>
+      <c r="Z114" s="39"/>
       <c r="AA114" s="39"/>
       <c r="AB114" s="39"/>
       <c r="AC114" s="39"/>
-      <c r="AD114" s="39" t="s">
-        <v>306</v>
-      </c>
+      <c r="AD114" s="39"/>
       <c r="AE114" s="39"/>
       <c r="AF114" s="39"/>
     </row>
@@ -9087,7 +8586,7 @@
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Z2:Z114 AE2:AE114</xm:sqref>
+          <xm:sqref>AE2:AE114 Z2:Z114</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{7E235E07-1A6D-41FA-8E32-72A730AFA7A4}">
           <x14:formula1>
@@ -9105,13 +8604,13 @@
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V114 AA2:AA114 AF2:AF114</xm:sqref>
+          <xm:sqref>V2:V114 AF2:AF114 AA2:AA114</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{192284F7-50B8-4585-A9B7-F422F5634CF8}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D07B0AA9-91AB-4733-9EAB-5035421C071A}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Y2:Y114 AD2:AD114</xm:sqref>
+          <xm:sqref>AD2:AD114 Y2:Y114</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9121,10 +8620,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F0DF1A-7900-47BA-8B9D-42C3E7E31390}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A2:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9136,230 +8635,228 @@
     <col min="7" max="7" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="F4" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="H5" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>246</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="N5" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5" s="38" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15">
+        <f>SUM(H6:O6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15">
+        <f>SUM(H7:O7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
-        <v>228</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>230</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>233</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="38" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15">
-        <f>SUM(C12:J12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15">
-        <f>SUM(C13:J13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15">
-        <f>SUM(C14:J14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
-        <v>236</v>
-      </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="37">
-        <f>SUM(K12:K14)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="57" t="s">
-        <v>257</v>
-      </c>
-      <c r="I16" s="57"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="35">
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15">
+        <f>SUM(H8:O8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="F9" s="52" t="s">
+        <v>251</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="37">
+        <f>SUM(P6:P8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F10" s="58" t="s">
+        <v>271</v>
+      </c>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="N10" s="56"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="35">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="59" t="s">
-        <v>255</v>
-      </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="38">
-        <f>SUM(K15:K16)</f>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="55" t="s">
+        <v>270</v>
+      </c>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="38">
+        <f>SUM(P9:P10)</f>
         <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A2:P2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:P4"/>
+    <mergeCell ref="F9:O9"/>
+    <mergeCell ref="F11:O11"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="F10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9382,70 +8879,70 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="A3" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
@@ -9464,7 +8961,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9476,7 +8973,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="39" t="s">
@@ -9487,14 +8984,15 @@
         <v>185</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="G1" s="47" t="s">
-        <v>305</v>
+      <c r="G1" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="C2" s="16"/>
       <c r="E2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -9506,8 +9004,8 @@
       <c r="E3" s="16">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>306</v>
+      <c r="G3" s="15" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9518,10 +9016,10 @@
         <v>29</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="G4" t="s">
-        <v>307</v>
+        <v>223</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -9534,22 +9032,22 @@
       <c r="E5" s="16">
         <v>8</v>
       </c>
-      <c r="G5" t="s">
-        <v>308</v>
+      <c r="G5" s="15" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" t="s">
-        <v>309</v>
+        <v>224</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -9565,12 +9063,12 @@
         <v>25</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="E9" s="16">
         <v>10</v>
@@ -9597,7 +9095,7 @@
         <v>24</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -9607,7 +9105,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="16" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -9616,8 +9114,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E16" s="48" t="s">
-        <v>213</v>
+      <c r="E16" s="46" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the excel data file templates. one has a macro that will generate the Shape Key field so the user does not need to do it. updated the user guide Added a new lookup table for Standard Stencil images Adjusted the excel data file template to use a look up so they don't need to know the name
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24CB03B4-57D1-4555-B967-17AD8A51FFC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9057D729-B1CE-4421-8804-6E9915A09F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27375" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9495" yWindow="1755" windowWidth="26505" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="325">
   <si>
     <t>Shape</t>
   </si>
@@ -1187,6 +1187,54 @@
   <si>
     <t>Dash_Dot</t>
   </si>
+  <si>
+    <t>Default Stencil Names</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Carousel2</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>EHRSystems</t>
+  </si>
+  <si>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>IconKey</t>
+  </si>
+  <si>
+    <t>IVX</t>
+  </si>
+  <si>
+    <t>Label1</t>
+  </si>
+  <si>
+    <t>NetworkPipe</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>TabelCell</t>
+  </si>
+  <si>
+    <t>vSuite_EMM</t>
+  </si>
+  <si>
+    <t>vSuiteCloud</t>
+  </si>
 </sst>
 </file>
 
@@ -1195,7 +1243,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1343,8 +1391,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1575,6 +1630,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1809,7 +1870,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1941,6 +2002,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1961,6 +2025,15 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="42" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2320,8 +2393,8 @@
   <dimension ref="A1:AF114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y92" sqref="Y92"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2360,16 +2433,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="61" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="62" t="s">
         <v>183</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -2411,10 +2484,10 @@
       <c r="Q1" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="63" t="s">
         <v>13</v>
       </c>
       <c r="T1" s="7" t="s">
@@ -2494,8 +2567,8 @@
       <c r="AF2" s="12"/>
     </row>
     <row r="3" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>293</v>
+      <c r="A3" s="16">
+        <v>0</v>
       </c>
       <c r="B3" s="44" t="s">
         <v>291</v>
@@ -2544,15 +2617,15 @@
       <c r="AF3" s="23"/>
     </row>
     <row r="4" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="39">
-        <v>0</v>
-      </c>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
         <v>299</v>
       </c>
       <c r="F4" s="21"/>
@@ -2592,17 +2665,17 @@
       <c r="AF4" s="23"/>
     </row>
     <row r="5" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>0</v>
-      </c>
-      <c r="B5" s="44" t="s">
+      <c r="A5" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="D5" s="17"/>
+      <c r="E5" s="17" t="s">
         <v>296</v>
       </c>
       <c r="F5" s="21"/>
@@ -2642,17 +2715,17 @@
       <c r="AF5" s="23"/>
     </row>
     <row r="6" spans="1:32" s="25" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
-        <v>0</v>
-      </c>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="19">
+        <v>0</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>297</v>
       </c>
       <c r="F6" s="21"/>
@@ -4361,7 +4434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="23">
         <v>1</v>
       </c>
@@ -4581,7 +4654,7 @@
       <c r="AE41" s="19"/>
       <c r="AF41" s="23"/>
     </row>
-    <row r="42" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
         <v>1</v>
       </c>
@@ -4645,7 +4718,7 @@
       <c r="AE42" s="19"/>
       <c r="AF42" s="23"/>
     </row>
-    <row r="43" spans="1:32" s="25" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
         <v>1</v>
       </c>
@@ -4777,7 +4850,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:32" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>133</v>
       </c>
@@ -8581,7 +8654,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{84DDF0C9-6F1B-446E-8995-2373E65B88E2}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
@@ -8612,6 +8685,12 @@
           </x14:formula1>
           <xm:sqref>AD2:AD114 Y2:Y114</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{000CBC19-A464-4694-A3AD-9D82A1CE6A27}">
+          <x14:formula1>
+            <xm:f>Tables!$I$2:$I$42</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D114</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -8636,24 +8715,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="36"/>
@@ -8662,25 +8741,25 @@
       <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="F4" s="51" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="F4" s="52" t="s">
         <v>243</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="51"/>
-      <c r="P4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
@@ -8794,55 +8873,55 @@
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="53" t="s">
         <v>251</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="53"/>
-      <c r="N9" s="53"/>
-      <c r="O9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="55"/>
       <c r="P9" s="37">
         <f>SUM(P6:P8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="59" t="s">
         <v>271</v>
       </c>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="56" t="s">
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="N10" s="56"/>
-      <c r="O10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="58"/>
       <c r="P10" s="35">
         <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="56" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="55"/>
       <c r="P11" s="38">
         <f>SUM(P9:P10)</f>
         <v>150</v>
@@ -8879,11 +8958,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="60" t="s">
         <v>252</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
@@ -8958,10 +9037,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0736EE8-23D0-4513-9563-3C6A65BAEEB4}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8969,9 +9048,10 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>288</v>
       </c>
@@ -8987,14 +9067,18 @@
       <c r="G1" s="45" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="42" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="C2" s="16"/>
       <c r="E2" s="16"/>
       <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>20</v>
       </c>
@@ -9007,8 +9091,11 @@
       <c r="G3" s="15" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
@@ -9021,8 +9108,11 @@
       <c r="G4" s="15" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="47" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>37</v>
       </c>
@@ -9035,8 +9125,11 @@
       <c r="G5" s="15" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>215</v>
       </c>
@@ -9049,73 +9142,236 @@
       <c r="G6" s="15" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="16">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="47" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>287</v>
       </c>
       <c r="E9" s="16">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="47" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="16">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="47" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="47" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" s="16">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="16" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="47" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="16">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="46" t="s">
         <v>228</v>
+      </c>
+      <c r="I16" s="47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="47" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="47" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="47" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="47" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="47" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="47" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="47" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="47" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="47" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="47" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="47" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="47" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="47" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -9123,7 +9379,7 @@
     <sortCondition ref="A3:A13"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:XFD2 B2:F2" xr:uid="{603106F1-35E4-4102-BBAC-864DFD6CCF25}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:F2 H2 J2:XFD2" xr:uid="{603106F1-35E4-4102-BBAC-864DFD6CCF25}">
       <formula1>$A$4:$A$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added Visio Page setup allowing the user to set orentation as well as page size via the Excel data file
</commit_message>
<xml_diff>
--- a/Data/ScriptData/Advocate_ArchitectData.xlsx
+++ b/Data/ScriptData/Advocate_ArchitectData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33951E34-AE72-4E66-B74F-E8F593D9B86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2486663E-B2A1-4847-B027-3EE9EA8A377F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20310" yWindow="1635" windowWidth="26505" windowHeight="15330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27630" yWindow="1170" windowWidth="26505" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="327">
   <si>
     <t>Shape</t>
   </si>
@@ -1227,13 +1227,19 @@
     <t>Title_Advocate</t>
   </si>
   <si>
-    <t>Custom</t>
-  </si>
-  <si>
     <t>Using a Visio Template that contains standard Stencils</t>
   </si>
   <si>
     <t>Account Custom Stencil</t>
+  </si>
+  <si>
+    <t>CustomerService</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>NetworkPipe3</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +1646,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1825,6 +1831,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1870,7 +1887,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2034,6 +2051,9 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2394,7 +2414,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,7 +2598,7 @@
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -2628,7 +2648,7 @@
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
@@ -8589,7 +8609,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{000CBC19-A464-4694-A3AD-9D82A1CE6A27}">
           <x14:formula1>
-            <xm:f>Tables!$I$2:$I$46</xm:f>
+            <xm:f>Tables!$I$2:$I$48</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D112</xm:sqref>
         </x14:dataValidation>
@@ -8939,10 +8959,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0736EE8-23D0-4513-9563-3C6A65BAEEB4}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9088,8 +9108,8 @@
       <c r="E10" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="I10" s="47" t="s">
-        <v>317</v>
+      <c r="I10" s="64" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -9100,7 +9120,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="47" t="s">
-        <v>18</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -9111,7 +9131,7 @@
         <v>224</v>
       </c>
       <c r="I12" s="47" t="s">
-        <v>303</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -9119,7 +9139,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -9127,7 +9147,7 @@
         <v>225</v>
       </c>
       <c r="I14" s="47" t="s">
-        <v>3</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -9135,168 +9155,175 @@
         <v>14</v>
       </c>
       <c r="I15" s="47" t="s">
-        <v>305</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="I16" s="47" t="s">
-        <v>87</v>
+      <c r="I16" s="64" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="47" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="47" t="s">
-        <v>320</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="47" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="47" t="s">
-        <v>89</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="47" t="s">
-        <v>308</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="47" t="s">
-        <v>34</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="47" t="s">
-        <v>1</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="47" t="s">
-        <v>309</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="47" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="47" t="s">
-        <v>11</v>
+        <v>309</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="47" t="s">
-        <v>310</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I29" s="47" t="s">
-        <v>4</v>
+      <c r="I29" s="64" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="47" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="47" t="s">
-        <v>94</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="47" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I33" s="47" t="s">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="47" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="47" t="s">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="47" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I35" s="47" t="s">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="47" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I36" s="47" t="s">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="47" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I37" s="47" t="s">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="47" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I38" s="47" t="s">
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="47" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I39" s="47" t="s">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="47" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="40" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I40" s="47" t="s">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="47" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I41" s="47" t="s">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="47" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="42" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I42" s="47" t="s">
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="47" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I43" s="47" t="s">
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I44" s="47" t="s">
+    <row r="47" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="47" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="45" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I45" s="47" t="s">
+    <row r="48" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="47" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I46" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="J46" t="s">
-        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>